<commit_message>
fix hot desk detail data bug
</commit_message>
<xml_diff>
--- a/backend/data/hot_desk_data.xlsx
+++ b/backend/data/hot_desk_data.xlsx
@@ -1,94 +1,401 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huoyingzhe/Documents/master课程/comp9900/project/backend/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C72DCB7-6408-E64C-ADF5-4E7A9DB3D750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="1140" windowWidth="27840" windowHeight="16940" xr2:uid="{FF493431-4319-1B40-968C-4E535F5285D6}"/>
+    <workbookView windowWidth="26080" windowHeight="13280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" calcCompleted="0" calcOnSave="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5">
   <si>
     <t>building</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
   </si>
   <si>
     <t>room</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>level</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>K17</t>
-  </si>
-  <si>
-    <t>K17</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
-      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -96,9 +403,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -107,17 +656,61 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -166,7 +759,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -199,26 +792,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -251,23 +827,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,26 +968,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC62A795-CF1A-D749-8642-419ED5006F72}">
-  <dimension ref="A1:D172"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133:A172"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="H206" sqref="H206"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" customWidth="1"/>
+    <col min="1" max="2" width="10.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -436,13 +990,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -461,7 +1015,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -926,10 +1480,10 @@
         <v>4</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -940,10 +1494,10 @@
         <v>4</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D37">
         <v>2</v>
@@ -954,10 +1508,10 @@
         <v>4</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -968,10 +1522,10 @@
         <v>4</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D39">
         <v>4</v>
@@ -982,10 +1536,10 @@
         <v>4</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D40">
         <v>5</v>
@@ -996,10 +1550,10 @@
         <v>4</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D41">
         <v>6</v>
@@ -1010,10 +1564,10 @@
         <v>4</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D42">
         <v>7</v>
@@ -1024,10 +1578,10 @@
         <v>4</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D43">
         <v>8</v>
@@ -1038,10 +1592,10 @@
         <v>4</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D44">
         <v>9</v>
@@ -1052,10 +1606,10 @@
         <v>4</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D45">
         <v>10</v>
@@ -1066,10 +1620,10 @@
         <v>4</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D46">
         <v>11</v>
@@ -1080,10 +1634,10 @@
         <v>4</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D47">
         <v>12</v>
@@ -1094,10 +1648,10 @@
         <v>4</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D48">
         <v>13</v>
@@ -1108,10 +1662,10 @@
         <v>4</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D49">
         <v>14</v>
@@ -1122,10 +1676,10 @@
         <v>4</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D50">
         <v>15</v>
@@ -1136,10 +1690,10 @@
         <v>4</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D51">
         <v>16</v>
@@ -1150,13 +1704,13 @@
         <v>4</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D52">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1164,13 +1718,13 @@
         <v>4</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53">
-        <v>301</v>
+        <v>217</v>
       </c>
       <c r="D53">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1184,7 +1738,7 @@
         <v>301</v>
       </c>
       <c r="D54">
-        <v>47</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1198,7 +1752,7 @@
         <v>301</v>
       </c>
       <c r="D55">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1212,7 +1766,7 @@
         <v>301</v>
       </c>
       <c r="D56">
-        <v>49</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1226,7 +1780,7 @@
         <v>301</v>
       </c>
       <c r="D57">
-        <v>50</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1234,13 +1788,13 @@
         <v>4</v>
       </c>
       <c r="B58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1248,13 +1802,13 @@
         <v>4</v>
       </c>
       <c r="B59">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C59">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1262,13 +1816,13 @@
         <v>4</v>
       </c>
       <c r="B60">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C60">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D60">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1276,13 +1830,13 @@
         <v>4</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D61">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1290,13 +1844,13 @@
         <v>4</v>
       </c>
       <c r="B62">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D62">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1304,13 +1858,13 @@
         <v>4</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D63">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1318,13 +1872,13 @@
         <v>4</v>
       </c>
       <c r="B64">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C64">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D64">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1332,13 +1886,13 @@
         <v>4</v>
       </c>
       <c r="B65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C65">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D65">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1346,13 +1900,13 @@
         <v>4</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C66">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D66">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1360,13 +1914,13 @@
         <v>4</v>
       </c>
       <c r="B67">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D67">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1374,13 +1928,13 @@
         <v>4</v>
       </c>
       <c r="B68">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C68">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D68">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1388,13 +1942,13 @@
         <v>4</v>
       </c>
       <c r="B69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D69">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1402,13 +1956,13 @@
         <v>4</v>
       </c>
       <c r="B70">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D70">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1416,13 +1970,13 @@
         <v>4</v>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D71">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1430,13 +1984,13 @@
         <v>4</v>
       </c>
       <c r="B72">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C72">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D72">
-        <v>15</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1444,13 +1998,13 @@
         <v>4</v>
       </c>
       <c r="B73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C73">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D73">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1458,13 +2012,13 @@
         <v>4</v>
       </c>
       <c r="B74">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C74">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D74">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1472,13 +2026,13 @@
         <v>4</v>
       </c>
       <c r="B75">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C75">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="D75">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1492,7 +2046,7 @@
         <v>401</v>
       </c>
       <c r="D76">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1506,7 +2060,7 @@
         <v>401</v>
       </c>
       <c r="D77">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1520,7 +2074,7 @@
         <v>401</v>
       </c>
       <c r="D78">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1534,7 +2088,7 @@
         <v>401</v>
       </c>
       <c r="D79">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1548,7 +2102,7 @@
         <v>401</v>
       </c>
       <c r="D80">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1562,7 +2116,7 @@
         <v>401</v>
       </c>
       <c r="D81">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1576,7 +2130,7 @@
         <v>401</v>
       </c>
       <c r="D82">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1590,7 +2144,7 @@
         <v>401</v>
       </c>
       <c r="D83">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1604,7 +2158,7 @@
         <v>401</v>
       </c>
       <c r="D84">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1618,7 +2172,7 @@
         <v>401</v>
       </c>
       <c r="D85">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1632,7 +2186,7 @@
         <v>401</v>
       </c>
       <c r="D86">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1646,7 +2200,7 @@
         <v>401</v>
       </c>
       <c r="D87">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1660,7 +2214,7 @@
         <v>401</v>
       </c>
       <c r="D88">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1674,7 +2228,7 @@
         <v>401</v>
       </c>
       <c r="D89">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1688,7 +2242,7 @@
         <v>401</v>
       </c>
       <c r="D90">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1702,7 +2256,7 @@
         <v>401</v>
       </c>
       <c r="D91">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1716,7 +2270,7 @@
         <v>401</v>
       </c>
       <c r="D92">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1730,7 +2284,7 @@
         <v>401</v>
       </c>
       <c r="D93">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1744,7 +2298,7 @@
         <v>401</v>
       </c>
       <c r="D94">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1758,7 +2312,7 @@
         <v>401</v>
       </c>
       <c r="D95">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1769,10 +2323,10 @@
         <v>4</v>
       </c>
       <c r="C96">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1783,10 +2337,10 @@
         <v>4</v>
       </c>
       <c r="C97">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D97">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1797,10 +2351,10 @@
         <v>4</v>
       </c>
       <c r="C98">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D98">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1811,10 +2365,10 @@
         <v>4</v>
       </c>
       <c r="C99">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D99">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1825,10 +2379,10 @@
         <v>4</v>
       </c>
       <c r="C100">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D100">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1839,10 +2393,10 @@
         <v>4</v>
       </c>
       <c r="C101">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D101">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1853,10 +2407,10 @@
         <v>4</v>
       </c>
       <c r="C102">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D102">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1867,10 +2421,10 @@
         <v>4</v>
       </c>
       <c r="C103">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D103">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1881,10 +2435,10 @@
         <v>4</v>
       </c>
       <c r="C104">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D104">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1895,10 +2449,10 @@
         <v>4</v>
       </c>
       <c r="C105">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D105">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1909,10 +2463,10 @@
         <v>4</v>
       </c>
       <c r="C106">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D106">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1923,10 +2477,10 @@
         <v>4</v>
       </c>
       <c r="C107">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D107">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1937,10 +2491,10 @@
         <v>4</v>
       </c>
       <c r="C108">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D108">
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1951,10 +2505,10 @@
         <v>4</v>
       </c>
       <c r="C109">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D109">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1965,10 +2519,10 @@
         <v>4</v>
       </c>
       <c r="C110">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D110">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -1979,10 +2533,10 @@
         <v>4</v>
       </c>
       <c r="C111">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="D111">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -1990,13 +2544,13 @@
         <v>4</v>
       </c>
       <c r="B112">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C112">
-        <v>501</v>
+        <v>401</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2004,13 +2558,13 @@
         <v>4</v>
       </c>
       <c r="B113">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C113">
-        <v>501</v>
+        <v>401</v>
       </c>
       <c r="D113">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2018,13 +2572,13 @@
         <v>4</v>
       </c>
       <c r="B114">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C114">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D114">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2032,13 +2586,13 @@
         <v>4</v>
       </c>
       <c r="B115">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C115">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D115">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2046,13 +2600,13 @@
         <v>4</v>
       </c>
       <c r="B116">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C116">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D116">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2060,13 +2614,13 @@
         <v>4</v>
       </c>
       <c r="B117">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C117">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D117">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2074,13 +2628,13 @@
         <v>4</v>
       </c>
       <c r="B118">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C118">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D118">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2088,13 +2642,13 @@
         <v>4</v>
       </c>
       <c r="B119">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C119">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D119">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2102,13 +2656,13 @@
         <v>4</v>
       </c>
       <c r="B120">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C120">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D120">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2116,13 +2670,13 @@
         <v>4</v>
       </c>
       <c r="B121">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C121">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D121">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2130,13 +2684,13 @@
         <v>4</v>
       </c>
       <c r="B122">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C122">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D122">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2144,13 +2698,13 @@
         <v>4</v>
       </c>
       <c r="B123">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C123">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D123">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2158,13 +2712,13 @@
         <v>4</v>
       </c>
       <c r="B124">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C124">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D124">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2172,13 +2726,13 @@
         <v>4</v>
       </c>
       <c r="B125">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C125">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D125">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2186,13 +2740,13 @@
         <v>4</v>
       </c>
       <c r="B126">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C126">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D126">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2200,13 +2754,13 @@
         <v>4</v>
       </c>
       <c r="B127">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C127">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D127">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2214,13 +2768,13 @@
         <v>4</v>
       </c>
       <c r="B128">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C128">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D128">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2228,13 +2782,13 @@
         <v>4</v>
       </c>
       <c r="B129">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C129">
-        <v>501</v>
+        <v>412</v>
       </c>
       <c r="D129">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2248,7 +2802,7 @@
         <v>501</v>
       </c>
       <c r="D130">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2262,7 +2816,7 @@
         <v>501</v>
       </c>
       <c r="D131">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2276,7 +2830,7 @@
         <v>501</v>
       </c>
       <c r="D132">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2290,7 +2844,7 @@
         <v>501</v>
       </c>
       <c r="D133">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2304,7 +2858,7 @@
         <v>501</v>
       </c>
       <c r="D134">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2318,7 +2872,7 @@
         <v>501</v>
       </c>
       <c r="D135">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2332,7 +2886,7 @@
         <v>501</v>
       </c>
       <c r="D136">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2346,7 +2900,7 @@
         <v>501</v>
       </c>
       <c r="D137">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2360,7 +2914,7 @@
         <v>501</v>
       </c>
       <c r="D138">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2374,7 +2928,7 @@
         <v>501</v>
       </c>
       <c r="D139">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2388,7 +2942,7 @@
         <v>501</v>
       </c>
       <c r="D140">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2402,7 +2956,7 @@
         <v>501</v>
       </c>
       <c r="D141">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2416,7 +2970,7 @@
         <v>501</v>
       </c>
       <c r="D142">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2430,7 +2984,7 @@
         <v>501</v>
       </c>
       <c r="D143">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2444,7 +2998,7 @@
         <v>501</v>
       </c>
       <c r="D144">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2458,7 +3012,7 @@
         <v>501</v>
       </c>
       <c r="D145">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2472,7 +3026,7 @@
         <v>501</v>
       </c>
       <c r="D146">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2486,7 +3040,7 @@
         <v>501</v>
       </c>
       <c r="D147">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2500,7 +3054,7 @@
         <v>501</v>
       </c>
       <c r="D148">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -2514,7 +3068,7 @@
         <v>501</v>
       </c>
       <c r="D149">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -2528,7 +3082,7 @@
         <v>501</v>
       </c>
       <c r="D150">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -2542,7 +3096,7 @@
         <v>501</v>
       </c>
       <c r="D151">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -2556,7 +3110,7 @@
         <v>501</v>
       </c>
       <c r="D152">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -2570,7 +3124,7 @@
         <v>501</v>
       </c>
       <c r="D153">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -2584,7 +3138,7 @@
         <v>501</v>
       </c>
       <c r="D154">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -2595,10 +3149,10 @@
         <v>5</v>
       </c>
       <c r="C155">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D155">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -2609,10 +3163,10 @@
         <v>5</v>
       </c>
       <c r="C156">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D156">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2623,10 +3177,10 @@
         <v>5</v>
       </c>
       <c r="C157">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D157">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2637,10 +3191,10 @@
         <v>5</v>
       </c>
       <c r="C158">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D158">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2651,10 +3205,10 @@
         <v>5</v>
       </c>
       <c r="C159">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D159">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2665,10 +3219,10 @@
         <v>5</v>
       </c>
       <c r="C160">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D160">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -2679,10 +3233,10 @@
         <v>5</v>
       </c>
       <c r="C161">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D161">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -2693,10 +3247,10 @@
         <v>5</v>
       </c>
       <c r="C162">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D162">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -2707,10 +3261,10 @@
         <v>5</v>
       </c>
       <c r="C163">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D163">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -2721,10 +3275,10 @@
         <v>5</v>
       </c>
       <c r="C164">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D164">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -2735,10 +3289,10 @@
         <v>5</v>
       </c>
       <c r="C165">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D165">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -2749,10 +3303,10 @@
         <v>5</v>
       </c>
       <c r="C166">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D166">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -2763,10 +3317,10 @@
         <v>5</v>
       </c>
       <c r="C167">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D167">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -2777,10 +3331,10 @@
         <v>5</v>
       </c>
       <c r="C168">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D168">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -2791,10 +3345,10 @@
         <v>5</v>
       </c>
       <c r="C169">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D169">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -2805,10 +3359,10 @@
         <v>5</v>
       </c>
       <c r="C170">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D170">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -2819,10 +3373,10 @@
         <v>5</v>
       </c>
       <c r="C171">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D171">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -2833,14 +3387,266 @@
         <v>5</v>
       </c>
       <c r="C172">
+        <v>501</v>
+      </c>
+      <c r="D172">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" t="s">
+        <v>4</v>
+      </c>
+      <c r="B173">
+        <v>5</v>
+      </c>
+      <c r="C173">
         <v>510</v>
       </c>
-      <c r="D172">
+      <c r="D173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" t="s">
+        <v>4</v>
+      </c>
+      <c r="B174">
+        <v>5</v>
+      </c>
+      <c r="C174">
+        <v>510</v>
+      </c>
+      <c r="D174">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" t="s">
+        <v>4</v>
+      </c>
+      <c r="B175">
+        <v>5</v>
+      </c>
+      <c r="C175">
+        <v>510</v>
+      </c>
+      <c r="D175">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" t="s">
+        <v>4</v>
+      </c>
+      <c r="B176">
+        <v>5</v>
+      </c>
+      <c r="C176">
+        <v>510</v>
+      </c>
+      <c r="D176">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" t="s">
+        <v>4</v>
+      </c>
+      <c r="B177">
+        <v>5</v>
+      </c>
+      <c r="C177">
+        <v>510</v>
+      </c>
+      <c r="D177">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" t="s">
+        <v>4</v>
+      </c>
+      <c r="B178">
+        <v>5</v>
+      </c>
+      <c r="C178">
+        <v>510</v>
+      </c>
+      <c r="D178">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" t="s">
+        <v>4</v>
+      </c>
+      <c r="B179">
+        <v>5</v>
+      </c>
+      <c r="C179">
+        <v>510</v>
+      </c>
+      <c r="D179">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" t="s">
+        <v>4</v>
+      </c>
+      <c r="B180">
+        <v>5</v>
+      </c>
+      <c r="C180">
+        <v>510</v>
+      </c>
+      <c r="D180">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" t="s">
+        <v>4</v>
+      </c>
+      <c r="B181">
+        <v>5</v>
+      </c>
+      <c r="C181">
+        <v>510</v>
+      </c>
+      <c r="D181">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" t="s">
+        <v>4</v>
+      </c>
+      <c r="B182">
+        <v>5</v>
+      </c>
+      <c r="C182">
+        <v>510</v>
+      </c>
+      <c r="D182">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" t="s">
+        <v>4</v>
+      </c>
+      <c r="B183">
+        <v>5</v>
+      </c>
+      <c r="C183">
+        <v>510</v>
+      </c>
+      <c r="D183">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" t="s">
+        <v>4</v>
+      </c>
+      <c r="B184">
+        <v>5</v>
+      </c>
+      <c r="C184">
+        <v>510</v>
+      </c>
+      <c r="D184">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" t="s">
+        <v>4</v>
+      </c>
+      <c r="B185">
+        <v>5</v>
+      </c>
+      <c r="C185">
+        <v>510</v>
+      </c>
+      <c r="D185">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" t="s">
+        <v>4</v>
+      </c>
+      <c r="B186">
+        <v>5</v>
+      </c>
+      <c r="C186">
+        <v>510</v>
+      </c>
+      <c r="D186">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" t="s">
+        <v>4</v>
+      </c>
+      <c r="B187">
+        <v>5</v>
+      </c>
+      <c r="C187">
+        <v>510</v>
+      </c>
+      <c r="D187">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" t="s">
+        <v>4</v>
+      </c>
+      <c r="B188">
+        <v>5</v>
+      </c>
+      <c r="C188">
+        <v>510</v>
+      </c>
+      <c r="D188">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" t="s">
+        <v>4</v>
+      </c>
+      <c r="B189">
+        <v>5</v>
+      </c>
+      <c r="C189">
+        <v>510</v>
+      </c>
+      <c r="D189">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" t="s">
+        <v>4</v>
+      </c>
+      <c r="B190">
+        <v>5</v>
+      </c>
+      <c r="C190">
+        <v>510</v>
+      </c>
+      <c r="D190">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>